<commit_message>
Actualiza titulo y reinicia asignaciones
</commit_message>
<xml_diff>
--- a/data/asignaciones.xlsx
+++ b/data/asignaciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,23 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2025-11-16T12:41:37</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>LINA MARIA FERNANDEZ</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>SAMUEL FELIPE CIRCA</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualiza listado de participantes y asignaciones
</commit_message>
<xml_diff>
--- a/data/asignaciones.xlsx
+++ b/data/asignaciones.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,499 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:39:26</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>LINA MARIA GARCIA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>AMPARO GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:41:50</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>CRISTIAN CAMILO PATIÑO</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>RAQUEL GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:41:58</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>MILENA ORJUELA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>JUAN DAVID GONZALEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:45:02</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LINA MARIA FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MILENA ORJUELA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:48:20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>CAROLINA ORJUELA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SAMUEL JOSE GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:49:35</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>CAMILO BARRETO</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SANTIAGO NOVA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:52:28</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ALVARO GARCIA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>FELISA GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:52:56</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>MARTHA SIERRA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MARIA JOSE GONZALEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-11-16T23:53:21</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>PAMELA GARCIA</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MONICA GONZALEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:03:06</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>JACOBO BARRETO</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO ROJAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:03:27</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TOMAS BARRETO</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>AURA MARIA PABON</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:06:53</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>AURA MARIA PABON</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>GLORIA GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:11:05</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>SAMUEL JOSE GARCIA</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ANGELA MARIA ROJAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:11:32</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>IVONNE ALARCON</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>SAMUEL FELIPE CIRCA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:14:37</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>CARLOS ALBERTO ROJAS</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SANDRA LILIANA ROJAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:15:28</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SANDRA LILIANA ROJAS</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>JOHANA CASTELBLANCO</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:16:06</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>ORIELSON ROJAS</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ESPERANZA GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:18:18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SANTIAGO NOVA</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>LINA MARIA FERNANDEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:19:30</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>GERARDO MORA</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>JULIANA GONZALEZ</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:21:05</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>FELISA GARCIA</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>LEONOR GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:21:21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>ANGELA MARIA ROJAS</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>MARTHA SIERRA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:24:44</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LUIS HENANDO ORJUELA</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ALVARO GARCIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:25:04</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>JERONIMO ORJUELA</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ERIKA ORJUELA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:25:30</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ERIKA ORJUELA</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>JERONIMO ORJUELA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:25:30</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>YOLANDA GARCIA</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ANDRES MONCADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:29:15</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>LEONOR GARCIA</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>TOMAS BARRETO</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:30:02</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ESPERANZA GARCIA</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>IVONNE ALARCON</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:32:28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>ALVARO CAMILO</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>JACOBO BARRETO</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-11-17T00:32:49</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>MONICA GONZALEZ</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>CAMILO BARRETO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>